<commit_message>
updates since july 30th
</commit_message>
<xml_diff>
--- a/June-Twitter-Corona.xlsx
+++ b/June-Twitter-Corona.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>2020-6-1</t>
   </si>
@@ -71,6 +71,45 @@
   </si>
   <si>
     <t>2020-6-17</t>
+  </si>
+  <si>
+    <t>2020-6-18</t>
+  </si>
+  <si>
+    <t>2020-6-19</t>
+  </si>
+  <si>
+    <t>2020-6-20</t>
+  </si>
+  <si>
+    <t>#COVIDIOTS: 20220</t>
+  </si>
+  <si>
+    <t>2020-6-21</t>
+  </si>
+  <si>
+    <t>2020-6-23</t>
+  </si>
+  <si>
+    <t>2020-6-24</t>
+  </si>
+  <si>
+    <t>2020-6-25</t>
+  </si>
+  <si>
+    <t>2020-6-26</t>
+  </si>
+  <si>
+    <t>2020-6-27</t>
+  </si>
+  <si>
+    <t>2020-6-28</t>
+  </si>
+  <si>
+    <t>2020-6-29</t>
+  </si>
+  <si>
+    <t>2020-6-30</t>
   </si>
 </sst>
 </file>
@@ -402,7 +441,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -542,11 +581,110 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>18</v>
       </c>
       <c r="B17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20">
+        <v>20220</v>
+      </c>
+      <c r="C20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29">
         <v>0</v>
       </c>
     </row>

</xml_diff>